<commit_message>
created new test file and updated layout for num columns
</commit_message>
<xml_diff>
--- a/src/data/ClueLayout.xlsx
+++ b/src/data/ClueLayout.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanlam/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanlam/eclipse-workspace/ClueGame/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66D38552-A11B-3C4B-8569-CE18FBAC8691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5777576-9BC7-1443-BB4B-E5BC1FED2C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -595,7 +595,7 @@
   <dimension ref="A1:AB29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC14" sqref="AC14"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3010,6 +3010,9 @@
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
       <c r="B29" s="3" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
adjusted layout filess and updated board initalization functions all fileinittests now pass
</commit_message>
<xml_diff>
--- a/src/data/ClueLayout.xlsx
+++ b/src/data/ClueLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dn990\OneDrive\Documents\csci306\ClueGame\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanlam/eclipse-workspace/ClueGame/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65402BF-E60A-4DD4-98E9-313A6F2E3BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFD822F-58C7-6342-B369-4D44C1FAC93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="-17790" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16460" yWindow="760" windowWidth="13780" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -598,13 +598,13 @@
       <selection activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="28" width="3" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2">
         <v>0</v>
       </c>
@@ -687,7 +687,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -773,7 +773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -859,7 +859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -945,7 +945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
implemented adjacency tests and some target tests
</commit_message>
<xml_diff>
--- a/src/data/ClueLayout.xlsx
+++ b/src/data/ClueLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanlam/eclipse-workspace/ClueGame/src/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dn990\OneDrive\Documents\csci306\ClueGame\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFD822F-58C7-6342-B369-4D44C1FAC93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14042F76-51F6-463D-A120-7993E7BA5A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16460" yWindow="760" windowWidth="13780" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14535" yWindow="-21600" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="42">
   <si>
     <t>X</t>
   </si>
@@ -131,6 +131,21 @@
   </si>
   <si>
     <t>W&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of doors:  26 </t>
+  </si>
+  <si>
+    <t>Dark Grey:  testAdjacencyDoor</t>
+  </si>
+  <si>
+    <t>Light Green: testAdjacenciesRooms</t>
+  </si>
+  <si>
+    <t>Dark Orange:  testAdjacencyWalkways</t>
+  </si>
+  <si>
+    <t>Dark Blue: test targets</t>
   </si>
 </sst>
 </file>
@@ -158,7 +173,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,18 +218,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -244,11 +271,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -284,7 +320,26 @@
     <xf numFmtId="3" fontId="1" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="1" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -592,19 +647,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AB29"/>
+  <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF3" sqref="AF3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AD9" sqref="AD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="28" width="3" style="10" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="35.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2">
         <v>0</v>
       </c>
@@ -686,8 +742,11 @@
       <c r="AB1" s="2">
         <v>26</v>
       </c>
+      <c r="AD1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -772,8 +831,11 @@
       <c r="AB2" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="AD2" s="19" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -858,8 +920,11 @@
       <c r="AB3" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="AD3" s="13" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="4" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -881,7 +946,7 @@
       <c r="G4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="12" t="s">
         <v>36</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -944,8 +1009,11 @@
       <c r="AB4" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="AD4" s="15" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="5" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -958,7 +1026,7 @@
       <c r="D5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="20" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -988,7 +1056,7 @@
       <c r="N5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="O5" s="18" t="s">
         <v>10</v>
       </c>
       <c r="P5" s="5" t="s">
@@ -1030,8 +1098,11 @@
       <c r="AB5" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="AD5" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="6" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1117,7 +1188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1203,7 +1274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1289,7 +1360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1375,7 +1446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1461,7 +1532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1547,7 +1618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1633,7 +1704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1719,7 +1790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1774,7 +1845,7 @@
       <c r="R14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="S14" s="4" t="s">
+      <c r="S14" s="14" t="s">
         <v>1</v>
       </c>
       <c r="T14" s="4" t="s">
@@ -1786,13 +1857,13 @@
       <c r="V14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="W14" s="13" t="s">
+      <c r="W14" s="8" t="s">
         <v>14</v>
       </c>
       <c r="X14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="Y14" s="12" t="s">
+      <c r="Y14" s="8" t="s">
         <v>17</v>
       </c>
       <c r="Z14" s="4" t="s">
@@ -1805,7 +1876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1891,7 +1962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1958,7 +2029,7 @@
       <c r="V16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="W16" s="7" t="s">
+      <c r="W16" s="17" t="s">
         <v>22</v>
       </c>
       <c r="X16" s="5" t="s">
@@ -1977,7 +2048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -2063,7 +2134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -2149,7 +2220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -2235,7 +2306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -2321,7 +2392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -2346,7 +2417,7 @@
       <c r="H21" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="I21" s="14" t="s">
         <v>1</v>
       </c>
       <c r="J21" s="4" t="s">
@@ -2407,7 +2478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -2420,7 +2491,7 @@
       <c r="D22" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F22" s="4" t="s">
@@ -2462,7 +2533,7 @@
       <c r="R22" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="S22" s="4" t="s">
+      <c r="S22" s="14" t="s">
         <v>1</v>
       </c>
       <c r="T22" s="4" t="s">
@@ -2493,7 +2564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -2579,7 +2650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -2665,7 +2736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -2705,7 +2776,7 @@
       <c r="M25" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="N25" s="7" t="s">
+      <c r="N25" s="20" t="s">
         <v>30</v>
       </c>
       <c r="O25" s="5" t="s">
@@ -2723,7 +2794,7 @@
       <c r="S25" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T25" s="8" t="s">
+      <c r="T25" s="12" t="s">
         <v>36</v>
       </c>
       <c r="U25" s="5" t="s">
@@ -2751,7 +2822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -2764,7 +2835,7 @@
       <c r="D26" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="20" t="s">
         <v>31</v>
       </c>
       <c r="F26" s="5" t="s">
@@ -2837,7 +2908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -2923,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -3009,7 +3080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -3031,7 +3102,7 @@
       <c r="G29" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="14" t="s">
         <v>1</v>
       </c>
       <c r="I29" s="3" t="s">

</xml_diff>

<commit_message>
added documentation for tests on spreadsheet
</commit_message>
<xml_diff>
--- a/src/data/ClueLayout.xlsx
+++ b/src/data/ClueLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dn990\OneDrive\Documents\csci306\ClueGame\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14042F76-51F6-463D-A120-7993E7BA5A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89E38A3-24A3-4471-BEDE-AD014B121EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14535" yWindow="-21600" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="44">
   <si>
     <t>X</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>Dark Blue: test targets</t>
+  </si>
+  <si>
+    <t>White: Door direction tests (FIleInitTests)</t>
+  </si>
+  <si>
+    <t>Light Grey: room tests (FileInitTests)</t>
   </si>
 </sst>
 </file>
@@ -173,7 +179,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,6 +246,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -284,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -340,6 +352,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -649,8 +673,8 @@
   </sheetPr>
   <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AD9" sqref="AD9"/>
+    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AD14" sqref="AD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -884,7 +908,7 @@
       <c r="P3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="23" t="s">
         <v>4</v>
       </c>
       <c r="R3" s="4" t="s">
@@ -967,7 +991,7 @@
       <c r="N4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="O4" s="24" t="s">
         <v>8</v>
       </c>
       <c r="P4" s="5" t="s">
@@ -1020,7 +1044,7 @@
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="23" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -1050,7 +1074,7 @@
       <c r="L5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="23" t="s">
         <v>3</v>
       </c>
       <c r="N5" s="5" t="s">
@@ -1080,7 +1104,7 @@
       <c r="V5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="W5" s="5" t="s">
+      <c r="W5" s="23" t="s">
         <v>5</v>
       </c>
       <c r="X5" s="7" t="s">
@@ -1273,6 +1297,7 @@
       <c r="AB7" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="AD7" s="21"/>
     </row>
     <row r="8" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -1359,6 +1384,9 @@
       <c r="AB8" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="AD8" s="21" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
@@ -1445,6 +1473,9 @@
       <c r="AB9" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="AD9" s="22" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="10" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
@@ -1602,7 +1633,7 @@
       <c r="W11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="X11" s="7" t="s">
+      <c r="X11" s="23" t="s">
         <v>18</v>
       </c>
       <c r="Y11" s="5" t="s">
@@ -1631,7 +1662,7 @@
       <c r="D12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="23" t="s">
         <v>19</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -1685,7 +1716,7 @@
       <c r="V12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="W12" s="5" t="s">
+      <c r="W12" s="23" t="s">
         <v>15</v>
       </c>
       <c r="X12" s="5" t="s">
@@ -2115,7 +2146,7 @@
       <c r="V17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="W17" s="5" t="s">
+      <c r="W17" s="23" t="s">
         <v>21</v>
       </c>
       <c r="X17" s="5" t="s">
@@ -2740,7 +2771,7 @@
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="23" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="5" t="s">
@@ -2770,7 +2801,7 @@
       <c r="K25" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="L25" s="23" t="s">
         <v>26</v>
       </c>
       <c r="M25" s="5" t="s">
@@ -2803,7 +2834,7 @@
       <c r="V25" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="W25" s="5" t="s">
+      <c r="W25" s="23" t="s">
         <v>27</v>
       </c>
       <c r="X25" s="5" t="s">

</xml_diff>

<commit_message>
updated adjtargettests and updated cluelayout
</commit_message>
<xml_diff>
--- a/src/data/ClueLayout.xlsx
+++ b/src/data/ClueLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dn990\OneDrive\Documents\csci306\ClueGame\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanlam/eclipse-workspace/ClueGame/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89E38A3-24A3-4471-BEDE-AD014B121EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3480AB1-B282-164A-B3CE-7719A26811BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14535" yWindow="-21600" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14740" yWindow="780" windowWidth="15500" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,7 +179,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,6 +252,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -296,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -354,7 +360,7 @@
     <xf numFmtId="3" fontId="1" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -364,6 +370,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -673,18 +683,18 @@
   </sheetPr>
   <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AD14" sqref="AD14"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="28" width="3" style="10" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="35.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2">
         <v>0</v>
       </c>
@@ -770,7 +780,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -859,7 +869,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -948,7 +958,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1037,7 +1047,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1059,7 +1069,7 @@
       <c r="G5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="26" t="s">
         <v>36</v>
       </c>
       <c r="I5" s="4" t="s">
@@ -1126,7 +1136,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1196,7 +1206,7 @@
       <c r="W6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="X6" s="7" t="s">
+      <c r="X6" s="26" t="s">
         <v>13</v>
       </c>
       <c r="Y6" s="5" t="s">
@@ -1212,7 +1222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1299,7 +1309,7 @@
       </c>
       <c r="AD7" s="21"/>
     </row>
-    <row r="8" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1388,7 +1398,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1401,7 +1411,7 @@
       <c r="D9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="26" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -1410,7 +1420,7 @@
       <c r="G9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="26" t="s">
         <v>1</v>
       </c>
       <c r="I9" s="4" t="s">
@@ -1477,7 +1487,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1563,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1624,7 +1634,7 @@
       <c r="T11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="U11" s="8" t="s">
+      <c r="U11" s="25" t="s">
         <v>11</v>
       </c>
       <c r="V11" s="5" t="s">
@@ -1649,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1735,7 +1745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1821,7 +1831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1891,7 +1901,7 @@
       <c r="W14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="X14" s="4" t="s">
+      <c r="X14" s="26" t="s">
         <v>1</v>
       </c>
       <c r="Y14" s="8" t="s">
@@ -1907,7 +1917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1993,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -2079,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -2165,7 +2175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -2251,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -2337,7 +2347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -2423,7 +2433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -2509,7 +2519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -2595,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -2681,7 +2691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -2767,7 +2777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -2853,7 +2863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -2939,7 +2949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -3025,7 +3035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -3111,7 +3121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
added color to gui
</commit_message>
<xml_diff>
--- a/src/data/ClueLayout.xlsx
+++ b/src/data/ClueLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanlam/eclipse-workspace/ClueGame/src/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dn990\OneDrive\Documents\csci306\ClueGame\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3480AB1-B282-164A-B3CE-7719A26811BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6536A686-6D73-4869-B802-49CBE7C357B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14740" yWindow="780" windowWidth="15500" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4680" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,7 +179,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,11 +198,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE59EDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
@@ -214,12 +209,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDCEAF7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -255,6 +244,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -325,24 +320,36 @@
     <xf numFmtId="3" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="2" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -354,26 +361,11 @@
     <xf numFmtId="3" fontId="2" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -684,17 +676,17 @@
   <dimension ref="A1:AD29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="28" width="3" style="10" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="28" width="3" style="9" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="35.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2">
         <v>0</v>
       </c>
@@ -780,7 +772,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -865,30 +857,30 @@
       <c r="AB2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AD2" s="19" t="s">
+      <c r="AD2" s="17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="25" t="s">
         <v>2</v>
       </c>
       <c r="H3" s="4" t="s">
@@ -903,22 +895,22 @@
       <c r="K3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="23" t="s">
+      <c r="Q3" s="21" t="s">
         <v>4</v>
       </c>
       <c r="R3" s="4" t="s">
@@ -933,54 +925,54 @@
       <c r="U3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="V3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="W3" s="5" t="s">
+      <c r="W3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="X3" s="5" t="s">
+      <c r="X3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="Y3" s="5" t="s">
+      <c r="Y3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="Z3" s="5" t="s">
+      <c r="Z3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AA3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="AB3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AD3" s="13" t="s">
+      <c r="AD3" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="10" t="s">
         <v>36</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -992,22 +984,22 @@
       <c r="K4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="25" t="s">
         <v>3</v>
       </c>
       <c r="R4" s="4" t="s">
@@ -1022,16 +1014,16 @@
       <c r="U4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="V4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="W4" s="5" t="s">
+      <c r="W4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="X4" s="5" t="s">
+      <c r="X4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="Y4" s="5" t="s">
+      <c r="Y4" s="25" t="s">
         <v>5</v>
       </c>
       <c r="Z4" s="3" t="s">
@@ -1043,33 +1035,33 @@
       <c r="AB4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AD4" s="15" t="s">
+      <c r="AD4" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="24" t="s">
         <v>36</v>
       </c>
       <c r="I5" s="4" t="s">
@@ -1081,22 +1073,22 @@
       <c r="K5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="23" t="s">
+      <c r="M5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="O5" s="18" t="s">
+      <c r="O5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="Q5" s="25" t="s">
         <v>3</v>
       </c>
       <c r="R5" s="4" t="s">
@@ -1108,54 +1100,54 @@
       <c r="T5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="U5" s="8" t="s">
+      <c r="U5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="V5" s="5" t="s">
+      <c r="V5" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="W5" s="23" t="s">
+      <c r="W5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="X5" s="7" t="s">
+      <c r="X5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Y5" s="5" t="s">
+      <c r="Y5" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="Z5" s="5" t="s">
+      <c r="Z5" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="AA5" s="5" t="s">
+      <c r="AA5" s="25" t="s">
         <v>5</v>
       </c>
       <c r="AB5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AD5" s="16" t="s">
+      <c r="AD5" s="14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="25" t="s">
         <v>2</v>
       </c>
       <c r="H6" s="4" t="s">
@@ -1170,22 +1162,22 @@
       <c r="K6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="P6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="Q6" s="5" t="s">
+      <c r="Q6" s="25" t="s">
         <v>3</v>
       </c>
       <c r="R6" s="4" t="s">
@@ -1197,32 +1189,32 @@
       <c r="T6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="U6" s="8" t="s">
+      <c r="U6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="V6" s="5" t="s">
+      <c r="V6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="W6" s="5" t="s">
+      <c r="W6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="X6" s="26" t="s">
+      <c r="X6" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="Y6" s="5" t="s">
+      <c r="Y6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="Z6" s="5" t="s">
+      <c r="Z6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="AA6" s="5" t="s">
+      <c r="AA6" s="25" t="s">
         <v>5</v>
       </c>
       <c r="AB6" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1262,10 +1254,10 @@
       <c r="M7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="N7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="O7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="P7" s="4" t="s">
@@ -1286,30 +1278,30 @@
       <c r="U7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="V7" s="5" t="s">
+      <c r="V7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="W7" s="5" t="s">
+      <c r="W7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="X7" s="5" t="s">
+      <c r="X7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="Y7" s="5" t="s">
+      <c r="Y7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="Z7" s="5" t="s">
+      <c r="Z7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="AA7" s="5" t="s">
+      <c r="AA7" s="25" t="s">
         <v>5</v>
       </c>
       <c r="AB7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AD7" s="21"/>
+      <c r="AD7" s="19"/>
     </row>
-    <row r="8" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1376,7 +1368,7 @@
       <c r="V8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="W8" s="8" t="s">
+      <c r="W8" s="7" t="s">
         <v>14</v>
       </c>
       <c r="X8" s="4" t="s">
@@ -1394,11 +1386,11 @@
       <c r="AB8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AD8" s="21" t="s">
+      <c r="AD8" s="19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1411,7 +1403,7 @@
       <c r="D9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="24" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -1420,7 +1412,7 @@
       <c r="G9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="26" t="s">
+      <c r="H9" s="24" t="s">
         <v>1</v>
       </c>
       <c r="I9" s="4" t="s">
@@ -1483,11 +1475,11 @@
       <c r="AB9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AD9" s="22" t="s">
+      <c r="AD9" s="20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1551,29 +1543,29 @@
       <c r="U10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="V10" s="5" t="s">
+      <c r="V10" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="W10" s="5" t="s">
+      <c r="W10" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="X10" s="7" t="s">
+      <c r="X10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="Y10" s="5" t="s">
+      <c r="Y10" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="Z10" s="5" t="s">
+      <c r="Z10" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="AA10" s="5" t="s">
+      <c r="AA10" s="25" t="s">
         <v>15</v>
       </c>
       <c r="AB10" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1586,7 +1578,7 @@
       <c r="D11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F11" s="4" t="s">
@@ -1634,32 +1626,32 @@
       <c r="T11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="U11" s="25" t="s">
+      <c r="U11" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="V11" s="5" t="s">
+      <c r="V11" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="W11" s="5" t="s">
+      <c r="W11" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="X11" s="23" t="s">
+      <c r="X11" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="Y11" s="5" t="s">
+      <c r="Y11" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="Z11" s="5" t="s">
+      <c r="Z11" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="AA11" s="5" t="s">
+      <c r="AA11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="AB11" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1669,16 +1661,16 @@
       <c r="C12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="5" t="s">
+      <c r="D12" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="25" t="s">
         <v>19</v>
       </c>
       <c r="H12" s="4" t="s">
@@ -1723,48 +1715,48 @@
       <c r="U12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="V12" s="5" t="s">
+      <c r="V12" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="W12" s="23" t="s">
+      <c r="W12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="X12" s="5" t="s">
+      <c r="X12" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="Y12" s="5" t="s">
+      <c r="Y12" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="Z12" s="5" t="s">
+      <c r="Z12" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="AA12" s="5" t="s">
+      <c r="AA12" s="25" t="s">
         <v>15</v>
       </c>
       <c r="AB12" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="5" t="s">
+      <c r="C13" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="25" t="s">
         <v>19</v>
       </c>
       <c r="H13" s="4" t="s">
@@ -1809,48 +1801,48 @@
       <c r="U13" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="V13" s="5" t="s">
+      <c r="V13" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="W13" s="5" t="s">
+      <c r="W13" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="X13" s="5" t="s">
+      <c r="X13" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="Y13" s="5" t="s">
+      <c r="Y13" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="Z13" s="5" t="s">
+      <c r="Z13" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="AA13" s="5" t="s">
+      <c r="AA13" s="25" t="s">
         <v>15</v>
       </c>
       <c r="AB13" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="7" t="s">
+      <c r="B14" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="5" t="s">
+      <c r="F14" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="25" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="4" t="s">
@@ -1886,7 +1878,7 @@
       <c r="R14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="S14" s="14" t="s">
+      <c r="S14" s="12" t="s">
         <v>1</v>
       </c>
       <c r="T14" s="4" t="s">
@@ -1898,13 +1890,13 @@
       <c r="V14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="W14" s="8" t="s">
+      <c r="W14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X14" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y14" s="8" t="s">
+      <c r="X14" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="7" t="s">
         <v>17</v>
       </c>
       <c r="Z14" s="4" t="s">
@@ -1917,26 +1909,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="B15" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="25" t="s">
         <v>19</v>
       </c>
       <c r="H15" s="4" t="s">
@@ -1981,51 +1973,51 @@
       <c r="U15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="V15" s="5" t="s">
+      <c r="V15" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="W15" s="5" t="s">
+      <c r="W15" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="X15" s="5" t="s">
+      <c r="X15" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="Y15" s="5" t="s">
+      <c r="Y15" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="Z15" s="5" t="s">
+      <c r="Z15" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AA15" s="5" t="s">
+      <c r="AA15" s="25" t="s">
         <v>21</v>
       </c>
       <c r="AB15" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="8" t="s">
+      <c r="B16" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>36</v>
       </c>
       <c r="I16" s="4" t="s">
@@ -2067,48 +2059,48 @@
       <c r="U16" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="V16" s="5" t="s">
+      <c r="V16" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="W16" s="17" t="s">
+      <c r="W16" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="X16" s="5" t="s">
+      <c r="X16" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="Y16" s="7" t="s">
+      <c r="Y16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Z16" s="5" t="s">
+      <c r="Z16" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AA16" s="5" t="s">
+      <c r="AA16" s="25" t="s">
         <v>21</v>
       </c>
       <c r="AB16" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="9" t="s">
+      <c r="B17" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="F17" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="25" t="s">
         <v>19</v>
       </c>
       <c r="H17" s="4" t="s">
@@ -2150,51 +2142,51 @@
       <c r="T17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="U17" s="8" t="s">
+      <c r="U17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="V17" s="5" t="s">
+      <c r="V17" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="W17" s="23" t="s">
+      <c r="W17" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="X17" s="5" t="s">
+      <c r="X17" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="Y17" s="5" t="s">
+      <c r="Y17" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="Z17" s="5" t="s">
+      <c r="Z17" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AA17" s="5" t="s">
+      <c r="AA17" s="25" t="s">
         <v>21</v>
       </c>
       <c r="AB17" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="5" t="s">
+      <c r="C18" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="25" t="s">
         <v>19</v>
       </c>
       <c r="H18" s="4" t="s">
@@ -2239,29 +2231,29 @@
       <c r="U18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="V18" s="5" t="s">
+      <c r="V18" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="W18" s="5" t="s">
+      <c r="W18" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="X18" s="5" t="s">
+      <c r="X18" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="Y18" s="5" t="s">
+      <c r="Y18" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="Z18" s="5" t="s">
+      <c r="Z18" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AA18" s="5" t="s">
+      <c r="AA18" s="25" t="s">
         <v>21</v>
       </c>
       <c r="AB18" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -2271,16 +2263,16 @@
       <c r="C19" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="5" t="s">
+      <c r="D19" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="25" t="s">
         <v>19</v>
       </c>
       <c r="H19" s="4" t="s">
@@ -2328,7 +2320,7 @@
       <c r="V19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="W19" s="8" t="s">
+      <c r="W19" s="7" t="s">
         <v>14</v>
       </c>
       <c r="X19" s="4" t="s">
@@ -2347,7 +2339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -2360,10 +2352,10 @@
       <c r="D20" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="4" t="s">
@@ -2433,7 +2425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -2458,7 +2450,7 @@
       <c r="H21" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I21" s="14" t="s">
+      <c r="I21" s="12" t="s">
         <v>1</v>
       </c>
       <c r="J21" s="4" t="s">
@@ -2519,7 +2511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -2532,7 +2524,7 @@
       <c r="D22" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F22" s="4" t="s">
@@ -2556,7 +2548,7 @@
       <c r="L22" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="M22" s="8" t="s">
+      <c r="M22" s="7" t="s">
         <v>17</v>
       </c>
       <c r="N22" s="4" t="s">
@@ -2565,7 +2557,7 @@
       <c r="O22" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="P22" s="8" t="s">
+      <c r="P22" s="7" t="s">
         <v>17</v>
       </c>
       <c r="Q22" s="4" t="s">
@@ -2574,7 +2566,7 @@
       <c r="R22" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="S22" s="14" t="s">
+      <c r="S22" s="12" t="s">
         <v>1</v>
       </c>
       <c r="T22" s="4" t="s">
@@ -2583,7 +2575,7 @@
       <c r="U22" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="V22" s="8" t="s">
+      <c r="V22" s="7" t="s">
         <v>17</v>
       </c>
       <c r="W22" s="4" t="s">
@@ -2592,7 +2584,7 @@
       <c r="X22" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="Y22" s="8" t="s">
+      <c r="Y22" s="7" t="s">
         <v>17</v>
       </c>
       <c r="Z22" s="4" t="s">
@@ -2605,7 +2597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -2615,16 +2607,16 @@
       <c r="C23" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G23" s="5" t="s">
+      <c r="D23" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="25" t="s">
         <v>25</v>
       </c>
       <c r="H23" s="4" t="s">
@@ -2633,84 +2625,84 @@
       <c r="I23" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="N23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="R23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="S23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T23" s="8" t="s">
+      <c r="J23" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="K23" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="L23" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="M23" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="N23" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="O23" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="P23" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q23" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="R23" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="S23" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="T23" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="U23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="V23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="W23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="X23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA23" s="5" t="s">
+      <c r="U23" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="V23" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="W23" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="X23" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y23" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z23" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA23" s="25" t="s">
         <v>27</v>
       </c>
       <c r="AB23" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="5" t="s">
+      <c r="B24" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="25" t="s">
         <v>25</v>
       </c>
       <c r="H24" s="4" t="s">
@@ -2719,170 +2711,170 @@
       <c r="I24" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="N24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="R24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="S24" s="5" t="s">
+      <c r="J24" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="K24" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="L24" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="M24" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="N24" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="O24" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="P24" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q24" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="R24" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="S24" s="25" t="s">
         <v>26</v>
       </c>
       <c r="T24" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="U24" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="V24" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="W24" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="X24" s="7" t="s">
+      <c r="U24" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="V24" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="W24" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="X24" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="Y24" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z24" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA24" s="5" t="s">
+      <c r="Y24" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z24" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA24" s="25" t="s">
         <v>27</v>
       </c>
       <c r="AB24" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="7" t="s">
+      <c r="B25" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H25" s="8" t="s">
+      <c r="E25" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="I25" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="J25" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L25" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="M25" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="N25" s="20" t="s">
+      <c r="J25" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="K25" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="L25" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="M25" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="N25" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="O25" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P25" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q25" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="R25" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="S25" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T25" s="12" t="s">
+      <c r="O25" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="P25" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q25" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="R25" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="S25" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="T25" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="U25" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="V25" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="W25" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="X25" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y25" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z25" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA25" s="5" t="s">
+      <c r="U25" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="V25" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="W25" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="X25" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y25" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z25" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA25" s="25" t="s">
         <v>27</v>
       </c>
       <c r="AB25" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E26" s="20" t="s">
+      <c r="B26" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" s="5" t="s">
+      <c r="F26" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="25" t="s">
         <v>25</v>
       </c>
       <c r="H26" s="4" t="s">
@@ -2891,84 +2883,84 @@
       <c r="I26" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="N26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="R26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="S26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T26" s="8" t="s">
+      <c r="J26" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="K26" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="L26" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="M26" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="N26" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="O26" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="P26" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q26" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="R26" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="S26" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="T26" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="U26" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="V26" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="W26" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="X26" s="7" t="s">
+      <c r="U26" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="V26" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="W26" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="X26" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="Y26" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z26" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA26" s="5" t="s">
+      <c r="Y26" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z26" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA26" s="25" t="s">
         <v>27</v>
       </c>
       <c r="AB26" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" s="5" t="s">
+      <c r="B27" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="25" t="s">
         <v>25</v>
       </c>
       <c r="H27" s="4" t="s">
@@ -2977,52 +2969,52 @@
       <c r="I27" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="N27" s="7" t="s">
+      <c r="J27" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="K27" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="L27" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="M27" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="N27" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="O27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="R27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="S27" s="5" t="s">
+      <c r="O27" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="P27" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q27" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="R27" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="S27" s="25" t="s">
         <v>26</v>
       </c>
       <c r="T27" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="U27" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="V27" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="W27" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="X27" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y27" s="6" t="s">
+      <c r="U27" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="V27" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="W27" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="X27" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y27" s="5" t="s">
         <v>34</v>
       </c>
       <c r="Z27" s="3" t="s">
@@ -3035,26 +3027,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" s="5" t="s">
+      <c r="C28" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="25" t="s">
         <v>25</v>
       </c>
       <c r="H28" s="4" t="s">
@@ -3063,10 +3055,10 @@
       <c r="I28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J28" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K28" s="5" t="s">
+      <c r="J28" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="K28" s="25" t="s">
         <v>26</v>
       </c>
       <c r="L28" s="3" t="s">
@@ -3087,25 +3079,25 @@
       <c r="Q28" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="R28" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="S28" s="5" t="s">
+      <c r="R28" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="S28" s="25" t="s">
         <v>26</v>
       </c>
       <c r="T28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="U28" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="V28" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="W28" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="X28" s="5" t="s">
+      <c r="U28" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="V28" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="W28" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="X28" s="25" t="s">
         <v>27</v>
       </c>
       <c r="Y28" s="3" t="s">
@@ -3121,29 +3113,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" s="5" t="s">
+      <c r="C29" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="25" t="s">
         <v>25</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H29" s="14" t="s">
+      <c r="H29" s="12" t="s">
         <v>1</v>
       </c>
       <c r="I29" s="3" t="s">

</xml_diff>

<commit_message>
added rooms, room labels, and door indications to boardpanel updated some locations of labels
</commit_message>
<xml_diff>
--- a/src/data/ClueLayout.xlsx
+++ b/src/data/ClueLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dn990\OneDrive\Documents\csci306\ClueGame\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanlam/eclipse-workspace/ClueGame/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6536A686-6D73-4869-B802-49CBE7C357B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDCF96E-3C9B-4C4A-8E5E-C0CA330A62FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4680" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="14000" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -675,18 +675,18 @@
   </sheetPr>
   <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="Z25" sqref="Z25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="28" width="3" style="9" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="35.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2">
         <v>0</v>
       </c>
@@ -772,7 +772,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -861,7 +861,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -950,7 +950,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1050,10 +1050,10 @@
         <v>2</v>
       </c>
       <c r="D5" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>2</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>9</v>
       </c>
       <c r="F5" s="25" t="s">
         <v>2</v>
@@ -1077,13 +1077,13 @@
         <v>3</v>
       </c>
       <c r="M5" s="21" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="N5" s="25" t="s">
         <v>3</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="P5" s="25" t="s">
         <v>3</v>
@@ -1128,7 +1128,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1196,10 +1196,10 @@
         <v>5</v>
       </c>
       <c r="W6" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="X6" s="24" t="s">
         <v>5</v>
-      </c>
-      <c r="X6" s="24" t="s">
-        <v>13</v>
       </c>
       <c r="Y6" s="25" t="s">
         <v>5</v>
@@ -1214,7 +1214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="AD7" s="19"/>
     </row>
-    <row r="8" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>15</v>
       </c>
       <c r="X11" s="21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="Y11" s="25" t="s">
         <v>15</v>
@@ -1651,7 +1651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>15</v>
       </c>
       <c r="W12" s="21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="X12" s="25" t="s">
         <v>15</v>
@@ -1737,7 +1737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1995,12 +1995,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>14</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>19</v>
@@ -2063,7 +2063,7 @@
         <v>21</v>
       </c>
       <c r="W16" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="X16" s="25" t="s">
         <v>21</v>
@@ -2081,7 +2081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>19</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F17" s="25" t="s">
         <v>19</v>
@@ -2146,7 +2146,7 @@
         <v>11</v>
       </c>
       <c r="V17" s="25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="W17" s="21" t="s">
         <v>21</v>
@@ -2167,7 +2167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>27</v>
       </c>
       <c r="X24" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="Y24" s="25" t="s">
         <v>27</v>
@@ -2769,7 +2769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>25</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F26" s="25" t="s">
         <v>25</v>
@@ -2920,13 +2920,13 @@
         <v>27</v>
       </c>
       <c r="V26" s="25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="W26" s="25" t="s">
         <v>27</v>
       </c>
       <c r="X26" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="Y26" s="25" t="s">
         <v>27</v>
@@ -2941,7 +2941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D27" s="25" t="s">
         <v>25</v>
@@ -3027,7 +3027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
corrected tests to reflect changes to room center and room label
</commit_message>
<xml_diff>
--- a/src/data/ClueLayout.xlsx
+++ b/src/data/ClueLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanlam/eclipse-workspace/ClueGame/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDCF96E-3C9B-4C4A-8E5E-C0CA330A62FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791F7B28-EBDC-4648-80E7-791B799277F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="14000" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -675,8 +675,8 @@
   </sheetPr>
   <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="Z25" sqref="Z25"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -964,7 +964,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F4" s="25" t="s">
         <v>2</v>
@@ -994,7 +994,7 @@
         <v>3</v>
       </c>
       <c r="O4" s="22" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="P4" s="25" t="s">
         <v>3</v>
@@ -1050,7 +1050,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>2</v>
@@ -1077,7 +1077,7 @@
         <v>3</v>
       </c>
       <c r="M5" s="21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N5" s="25" t="s">
         <v>3</v>
@@ -1110,7 +1110,7 @@
         <v>5</v>
       </c>
       <c r="X5" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Y5" s="25" t="s">
         <v>5</v>
@@ -1196,7 +1196,7 @@
         <v>5</v>
       </c>
       <c r="W6" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="X6" s="24" t="s">
         <v>5</v>
@@ -1550,7 +1550,7 @@
         <v>15</v>
       </c>
       <c r="X10" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="Y10" s="25" t="s">
         <v>15</v>
@@ -1719,7 +1719,7 @@
         <v>15</v>
       </c>
       <c r="W12" s="21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="X12" s="25" t="s">
         <v>15</v>
@@ -1837,7 +1837,7 @@
         <v>19</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F14" s="25" t="s">
         <v>19</v>
@@ -2000,7 +2000,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>19</v>
@@ -2060,7 +2060,7 @@
         <v>1</v>
       </c>
       <c r="V16" s="25" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="W16" s="15" t="s">
         <v>21</v>
@@ -2069,7 +2069,7 @@
         <v>21</v>
       </c>
       <c r="Y16" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Z16" s="25" t="s">
         <v>21</v>
@@ -2146,13 +2146,13 @@
         <v>11</v>
       </c>
       <c r="V17" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W17" s="21" t="s">
         <v>21</v>
       </c>
       <c r="X17" s="25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y17" s="25" t="s">
         <v>21</v>
@@ -2754,7 +2754,7 @@
         <v>27</v>
       </c>
       <c r="X24" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Y24" s="25" t="s">
         <v>27</v>
@@ -2780,7 +2780,7 @@
         <v>25</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>25</v>
@@ -2810,7 +2810,7 @@
         <v>26</v>
       </c>
       <c r="N25" s="18" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="O25" s="25" t="s">
         <v>26</v>
@@ -2920,7 +2920,7 @@
         <v>27</v>
       </c>
       <c r="V26" s="25" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="W26" s="25" t="s">
         <v>27</v>
@@ -2949,7 +2949,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D27" s="25" t="s">
         <v>25</v>
@@ -2982,7 +2982,7 @@
         <v>26</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O27" s="25" t="s">
         <v>26</v>

</xml_diff>